<commit_message>
create js files and edit days_until_end.py templatetag
</commit_message>
<xml_diff>
--- a/media/raporty.xlsx
+++ b/media/raporty.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,26 +609,93 @@
         <v>160</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-08-12</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>160</v>
+      </c>
+    </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>RAZEM:</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>320</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+          <t>2023-08-10</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>16:0</t>
+          <t>8:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0:00</t>
+          <t>00.00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -645,9 +712,896 @@
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>320</v>
-      </c>
-      <c r="N6" t="inlineStr"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-08-09</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-08-08</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-08-07</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Test1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>7:30</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-08-15</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Test 3</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>7:30</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-08-14</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Test 3</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>7:30</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-08-11</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Test 3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>7:15</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-08-08</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Test 3</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>7:30</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>20</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>80</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-08-09</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Test 3</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0:30</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-08-24</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Test 3</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-08-15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>20</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>80</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-08-24</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>6:00</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-08-25</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Test 5</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>7:30</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023-08-23</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023-09-01</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023-10-04</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Test 1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>8:00</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>00.00</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>RAZEM:</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>3305</v>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>155:15</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0:30</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>40</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>160</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>3105</v>
+      </c>
+      <c r="N24" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>